<commit_message>
alteracoes do endereco do txt de edicao, criacao da vinheta de inicio, readme com codigo de corte
</commit_message>
<xml_diff>
--- a/arquivos/parametros/Modelo_Parametros.xlsx
+++ b/arquivos/parametros/Modelo_Parametros.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felyppe\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA9CC2-CE53-4B63-BE4D-64ACD79A368E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1680" windowWidth="29040" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Corte" sheetId="1" r:id="rId1"/>
     <sheet name="Merge" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,13 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>./arquivos/sem_edicao/preparacao_ambiente.mp4</t>
-  </si>
-  <si>
-    <t>final-aula1.mp4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Nome_Final_Arquivo</t>
   </si>
@@ -50,9 +38,6 @@
     <t>Minuto_Corte</t>
   </si>
   <si>
-    <t>5:00.00</t>
-  </si>
-  <si>
     <t>Nome_Arquivo</t>
   </si>
   <si>
@@ -81,12 +66,24 @@
   </si>
   <si>
     <t>./arquivos/sem_edicao/Aula 15 - C# - Estrutura de Repetição_PT1.mp4;./arquivos/sem_edicao/Aula 15 - C# - Estrutura de Repetição_PT2.mp4;Aula 15 - C# - Estrutura de Repetição.mp4</t>
+  </si>
+  <si>
+    <t>M-AlgoJS - Algoritmos.mp4</t>
+  </si>
+  <si>
+    <t>00:04.00</t>
+  </si>
+  <si>
+    <t>./arquivos/sem_edicao/Aula01.mp4</t>
+  </si>
+  <si>
+    <t>./arquivos/sem_edicao/Aula01.mp4;00:04.00;M-AlgoJS - Algoritmos.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,50 +387,58 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="107.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2,";",B2,";",C2)</f>
+        <v>./arquivos/sem_edicao/Aula01.mp4;00:04.00;M-AlgoJS - Algoritmos.mp4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -442,57 +447,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF68A565-CEE0-43B8-B15D-FE6D9B91E93A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="162.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="162.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE(A2,B2,";",A2,C2,";",D2)</f>
         <v>./arquivos/sem_edicao/Aula 15 - C# - Estrutura de Repetição_PT1.mp4;./arquivos/sem_edicao/Aula 15 - C# - Estrutura de Repetição_PT2.mp4;Aula 15 - C# - Estrutura de Repetição.mp4</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>